<commit_message>
Added Employer Integration Tests
</commit_message>
<xml_diff>
--- a/src/Sfa.Tl.Matching.Application.IntegrationTests/Employer/Employer-Simple.xlsx
+++ b/src/Sfa.Tl.Matching.Application.IntegrationTests/Employer/Employer-Simple.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\Esfa\tl-matching\src\Sfa.Tl.Matching.FileReader.Excel.IntegrationTests\Employer\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\DFE\tl-matching\src\Sfa.Tl.Matching.Application.IntegrationTests\Employer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AE05324-43CE-4A99-8A02-FE065F00ABEF}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F709149-D9B7-49B7-B158-593747DC3A58}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Account Advanced Find View" sheetId="1" r:id="rId1"/>
     <sheet name="hiddenSheet" sheetId="2" state="veryHidden" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="27">
   <si>
     <t>(Do Not Modify) Account</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>email@address.com</t>
+  </si>
+  <si>
+    <t>CompanyType</t>
   </si>
 </sst>
 </file>
@@ -171,15 +174,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:K2" totalsRowShown="0">
-  <autoFilter ref="A1:K2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="11">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:L2" totalsRowShown="0">
+  <autoFilter ref="A1:L2" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="12">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="(Do Not Modify) Account"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="(Do Not Modify) Row Checksum"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="(Do Not Modify) Modified On"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Company Name"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Also Known As"/>
     <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="AUPA"/>
+    <tableColumn id="7" xr3:uid="{3415DACA-03AA-4602-84EC-6FA700F2C741}" name="CompanyType"/>
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Primary Contact"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Main Phone"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Email" dataCellStyle="Hyperlink"/>
@@ -488,28 +492,29 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="dataSheet"/>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="0" style="1" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="46.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="42.42578125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="42" style="4" customWidth="1"/>
-    <col min="5" max="5" width="14" style="5" customWidth="1"/>
-    <col min="6" max="6" width="14" style="6" customWidth="1"/>
-    <col min="7" max="7" width="21" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14" style="8" customWidth="1"/>
-    <col min="9" max="9" width="14" style="9" customWidth="1"/>
-    <col min="10" max="10" width="14" style="10" customWidth="1"/>
-    <col min="11" max="11" width="14" style="11" customWidth="1"/>
+    <col min="1" max="1" width="35.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" style="10" customWidth="1"/>
+    <col min="8" max="8" width="16.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.44140625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.77734375" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.6640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.77734375" style="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -528,23 +533,26 @@
       <c r="F1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="11" t="s">
+        <v>26</v>
+      </c>
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
+    <row r="2" spans="1:12">
       <c r="A2" s="1" t="s">
         <v>11</v>
       </c>
@@ -563,19 +571,22 @@
       <c r="F2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="11">
+      <c r="I2" s="11">
         <v>7777744465</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K2" s="11" t="s">
+      <c r="L2" s="11" t="s">
         <v>10</v>
       </c>
     </row>
@@ -590,20 +601,20 @@
     <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 100 characters long." promptTitle="Text" prompt="Maximum Length: 100 characters." sqref="E2:E1048576" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>100</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Primary Contact record must already exist in Microsoft Dynamics CRM or in this source file." sqref="G2:G1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 55 characters long." promptTitle="Text" prompt="Maximum Length: 55 characters." sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup" prompt="This Primary Contact record must already exist in Microsoft Dynamics CRM or in this source file." sqref="H2:H1048576" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 55 characters long." promptTitle="Text" prompt="Maximum Length: 55 characters." sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000006000000}">
       <formula1>55</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 159 characters long." promptTitle="Text" prompt="Maximum Length: 159 characters." sqref="I2:I1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 159 characters long." promptTitle="Text" prompt="Maximum Length: 159 characters." sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0000-000007000000}">
       <formula1>159</formula1>
     </dataValidation>
-    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 8 characters long." promptTitle="Text (required)" prompt="Maximum Length: 8 characters." sqref="J2:J1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
+    <dataValidation type="textLength" operator="lessThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Length Exceeded" error="This value must be less than or equal to 8 characters long." promptTitle="Text (required)" prompt="Maximum Length: 8 characters." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-00000C000000}">
       <formula1>8</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics CRM or in this source file." sqref="K2:K1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" error=" " promptTitle="Lookup (required)" prompt="This Owner record must already exist in Microsoft Dynamics CRM or in this source file." sqref="L2:L1048576" xr:uid="{00000000-0002-0000-0000-000011000000}"/>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="I2" r:id="rId1" xr:uid="{7A3CD807-0926-4B9D-8950-B6D78E3B1357}"/>
+    <hyperlink ref="J2" r:id="rId1" xr:uid="{7A3CD807-0926-4B9D-8950-B6D78E3B1357}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
@@ -617,7 +628,7 @@
           <x14:formula1>
             <xm:f>hiddenSheet!$A$2:$D$2</xm:f>
           </x14:formula1>
-          <xm:sqref>F2:F1048576</xm:sqref>
+          <xm:sqref>F2:F1048576 G3:G1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -632,7 +643,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">

</xml_diff>